<commit_message>
Published state of ETDataset on 29 Sept 2022
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/transport/transport_ship_using_hydrogen.xlsx
+++ b/nodes_source_analyses/energy/transport/transport_ship_using_hydrogen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/nodes_source_analyses/energy/transport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34E4D74-3E06-144E-A2FB-C21E75EE7C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2DA21A-F745-7E47-B5E0-57E0BA42B59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27140" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
   <si>
     <t>Source</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>CE Delft, CO2 emissiefactoren, Smartport, Interreg</t>
+  </si>
+  <si>
+    <t>Quintel assumption</t>
   </si>
 </sst>
 </file>
@@ -339,12 +342,19 @@
     <numFmt numFmtId="167" formatCode="0.000000000"/>
     <numFmt numFmtId="168" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -800,452 +810,454 @@
   </borders>
   <cellStyleXfs count="248">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="177" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="14" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="177" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="177" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="177" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="248">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2504,7 +2516,7 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -2690,8 +2702,8 @@
   </sheetPr>
   <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
@@ -2716,36 +2728,36 @@
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="120"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="124"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="121"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="123"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="127"/>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="121"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="123"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="127"/>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="124"/>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="126"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="130"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
     </row>
@@ -2825,8 +2837,8 @@
         <v>42</v>
       </c>
       <c r="H11" s="27"/>
-      <c r="I11" s="78" t="s">
-        <v>47</v>
+      <c r="I11" s="132" t="s">
+        <v>86</v>
       </c>
       <c r="J11" s="13"/>
     </row>
@@ -2846,7 +2858,9 @@
         <v>43</v>
       </c>
       <c r="H12" s="34"/>
-      <c r="I12" s="78"/>
+      <c r="I12" s="133" t="s">
+        <v>87</v>
+      </c>
       <c r="J12" s="68"/>
       <c r="K12" s="31"/>
     </row>
@@ -2926,7 +2940,7 @@
   <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
@@ -3014,7 +3028,7 @@
       </c>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
-      <c r="I7" s="131" t="s">
+      <c r="I7" s="121" t="s">
         <v>86</v>
       </c>
       <c r="J7" s="44"/>
@@ -3207,7 +3221,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="86"/>
-      <c r="C8" s="129" t="s">
+      <c r="C8" s="119" t="s">
         <v>78</v>
       </c>
       <c r="D8" s="80" t="s">
@@ -3321,13 +3335,13 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="86"/>
-      <c r="C17" s="129" t="s">
+      <c r="C17" s="119" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="128" t="s">
+      <c r="D17" s="118" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="128" t="s">
+      <c r="E17" s="118" t="s">
         <v>82</v>
       </c>
       <c r="F17" s="103">
@@ -3337,7 +3351,7 @@
         <v>44746</v>
       </c>
       <c r="I17" s="80"/>
-      <c r="J17" s="130" t="s">
+      <c r="J17" s="120" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3354,13 +3368,13 @@
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="86"/>
-      <c r="C20" s="128" t="s">
+      <c r="C20" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="128" t="s">
+      <c r="D20" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="128" t="s">
+      <c r="E20" s="118" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="80">
@@ -3369,7 +3383,7 @@
       <c r="H20" s="104">
         <v>44746</v>
       </c>
-      <c r="J20" s="130" t="s">
+      <c r="J20" s="120" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3408,7 +3422,7 @@
   </sheetPr>
   <dimension ref="A1:Q124"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
@@ -3606,34 +3620,34 @@
       <c r="G24" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="127" t="s">
+      <c r="H24" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="I24" s="127"/>
-      <c r="J24" s="127"/>
-      <c r="K24" s="127"/>
-      <c r="L24" s="127"/>
-      <c r="M24" s="127"/>
+      <c r="I24" s="131"/>
+      <c r="J24" s="131"/>
+      <c r="K24" s="131"/>
+      <c r="L24" s="131"/>
+      <c r="M24" s="131"/>
       <c r="Q24" s="87"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="86"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-      <c r="K25" s="127"/>
-      <c r="L25" s="127"/>
-      <c r="M25" s="127"/>
+      <c r="H25" s="131"/>
+      <c r="I25" s="131"/>
+      <c r="J25" s="131"/>
+      <c r="K25" s="131"/>
+      <c r="L25" s="131"/>
+      <c r="M25" s="131"/>
       <c r="Q25" s="87"/>
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="86"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-      <c r="K26" s="127"/>
-      <c r="L26" s="127"/>
-      <c r="M26" s="127"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="131"/>
       <c r="Q26" s="87"/>
     </row>
     <row r="27" spans="2:17">
@@ -3642,7 +3656,7 @@
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="86"/>
-      <c r="E28" s="128" t="s">
+      <c r="E28" s="118" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="89">
@@ -3652,7 +3666,7 @@
       <c r="G28" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="128" t="s">
+      <c r="H28" s="118" t="s">
         <v>76</v>
       </c>
       <c r="Q28" s="87"/>
@@ -3900,22 +3914,22 @@
     </row>
     <row r="65" spans="2:17">
       <c r="B65" s="86"/>
-      <c r="C65" s="128" t="s">
+      <c r="C65" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="128" t="s">
+      <c r="D65" s="118" t="s">
         <v>70</v>
       </c>
       <c r="Q65" s="87"/>
     </row>
     <row r="66" spans="2:17">
       <c r="B66" s="86"/>
-      <c r="D66" s="128"/>
+      <c r="D66" s="118"/>
       <c r="Q66" s="87"/>
     </row>
     <row r="67" spans="2:17">
       <c r="B67" s="86"/>
-      <c r="D67" s="128" t="s">
+      <c r="D67" s="118" t="s">
         <v>71</v>
       </c>
       <c r="Q67" s="87"/>
@@ -3978,47 +3992,47 @@
     </row>
     <row r="81" spans="2:17">
       <c r="B81" s="86"/>
-      <c r="C81" s="128" t="s">
+      <c r="C81" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="D81" s="128" t="s">
+      <c r="D81" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="E81" s="128" t="s">
+      <c r="E81" s="118" t="s">
         <v>75</v>
       </c>
       <c r="F81" s="80">
         <f>0.45/0.42</f>
         <v>1.0714285714285714</v>
       </c>
-      <c r="G81" s="128" t="s">
+      <c r="G81" s="118" t="s">
         <v>72</v>
       </c>
-      <c r="H81" s="128" t="s">
+      <c r="H81" s="118" t="s">
         <v>73</v>
       </c>
       <c r="Q81" s="87"/>
     </row>
     <row r="82" spans="2:17">
       <c r="B82" s="86"/>
-      <c r="H82" s="128" t="s">
+      <c r="H82" s="118" t="s">
         <v>74</v>
       </c>
       <c r="Q82" s="87"/>
     </row>
     <row r="83" spans="2:17">
       <c r="B83" s="86"/>
-      <c r="E83" s="128" t="s">
+      <c r="E83" s="118" t="s">
         <v>79</v>
       </c>
       <c r="F83" s="80">
         <f>F28*F81</f>
         <v>3.4013605442176869</v>
       </c>
-      <c r="G83" s="128" t="s">
+      <c r="G83" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="H83" s="128" t="s">
+      <c r="H83" s="118" t="s">
         <v>77</v>
       </c>
       <c r="Q83" s="87"/>

</xml_diff>